<commit_message>
made updates to index etc
</commit_message>
<xml_diff>
--- a/data/home_data.xlsx
+++ b/data/home_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vipin\New Volume\prasad-research.github.io\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prasad-research.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB28F2-30C0-4807-A140-99D681C39479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495E34B0-CFA8-4A01-9C2D-EFDDDD07B4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="News" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -40,9 +40,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>Our research on xyz has been accepted at a top-tier conference!</t>
-  </si>
-  <si>
     <t>Badge</t>
   </si>
   <si>
@@ -52,13 +49,22 @@
     <t>Authors</t>
   </si>
   <si>
-    <t>Paper Title</t>
-  </si>
-  <si>
-    <t>first name, last name, firstname lastname</t>
-  </si>
-  <si>
-    <t>AAAI</t>
+    <t>Rish Prakash (SMVDU Katra; Intern at IIT Goa), Dr. Anuj Abraham (Research Fellow, IIT Goa), and Dr. Shitala Prasad (Assistant Professor, IIT Goa) on receiving the Best Application Paper Award at the International Intelligent Computing and Technology Conference (ICTCon) 2025, held on 2–3 December 2025. Their award-winning paper, “Hybrid Multi-view 3D Object Detection from 2D Images: Fusion of Structure-from-Motion and Learned Depth Priors,” showcases impactful research and innovation in the field of intelligent computing and computer vision</t>
+  </si>
+  <si>
+    <t>https://ictcon2025.cit.ac.in/</t>
+  </si>
+  <si>
+    <t>[Student Achievement] Vipin Gautam, PhD student in the Department of Computer Science and Engineering, received the Best Oral Presentation Award at the Goa Research Scholars Meet 2025, organized by the Centre for Research, Development &amp; Innovation (RDI), Department of Higher Education, Goa, on 20–21 November 2025. He presented his work titled “Bridging RGB–IR Domains for Aerial Object Detection.” Vipin is supervised by Dr. Shitala Prasad, Assistant Professor, Computer Science and Engineering and Dr. Sharad Sinha, Associate Professor, Computer Science and Engineering.</t>
+  </si>
+  <si>
+    <t>IEEE SPL</t>
+  </si>
+  <si>
+    <t>SequenceOut: Boosting CNNs by Freezing Layers</t>
+  </si>
+  <si>
+    <t>S Prasad, R Paul, M Kamat</t>
   </si>
 </sst>
 </file>
@@ -379,13 +385,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -402,21 +409,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -431,21 +438,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC5C1AF-0258-426F-AF24-056AA985BE35}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,13 +460,14 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>